<commit_message>
Circuit Format Change and ChipDesignGraph Class Creation and some minor bugs are resolved
</commit_message>
<xml_diff>
--- a/DeepRL/Data/stdcell45nm.xlsx
+++ b/DeepRL/Data/stdcell45nm.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\Projects\Automate Chip Design Using ML and DL\Model Work\DeepRL\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AB7A6E20-7469-4B6B-B71B-82D4E27D8F40}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F2344E5E-CF84-4893-9C73-E1E41E936767}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,72 +25,36 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="22">
-  <si>
-    <t>BUF2</t>
-  </si>
-  <si>
-    <t>NOT</t>
-  </si>
-  <si>
-    <t>AND2</t>
-  </si>
-  <si>
-    <t>NAND2</t>
-  </si>
-  <si>
-    <t>NAND3</t>
-  </si>
-  <si>
-    <t>AND3</t>
-  </si>
-  <si>
-    <t>NOR2</t>
-  </si>
-  <si>
-    <t>AND4</t>
-  </si>
-  <si>
-    <t>NAND4</t>
-  </si>
-  <si>
-    <t>OR3</t>
-  </si>
-  <si>
-    <t>NOR3</t>
-  </si>
-  <si>
-    <t>AND5</t>
-  </si>
-  <si>
-    <t>NOR8</t>
-  </si>
-  <si>
-    <t>OR4</t>
-  </si>
-  <si>
-    <t>NOR4</t>
-  </si>
-  <si>
-    <t>AND9</t>
-  </si>
-  <si>
-    <t>OR2</t>
-  </si>
-  <si>
-    <t>BUF4</t>
-  </si>
-  <si>
-    <t>DFFPOS</t>
-  </si>
-  <si>
-    <t>DFFNEG</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
   <si>
     <t>MACROS</t>
   </si>
   <si>
     <t>AREA</t>
+  </si>
+  <si>
+    <t>nand</t>
+  </si>
+  <si>
+    <t>or</t>
+  </si>
+  <si>
+    <t>buf</t>
+  </si>
+  <si>
+    <t>not</t>
+  </si>
+  <si>
+    <t>and</t>
+  </si>
+  <si>
+    <t>nor</t>
+  </si>
+  <si>
+    <t>dffpos</t>
+  </si>
+  <si>
+    <t>dffneg</t>
   </si>
 </sst>
 </file>
@@ -408,187 +372,83 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:B22"/>
+  <dimension ref="A1:B9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D4" sqref="D4"/>
+      <selection activeCell="B13" sqref="B13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
-        <v>20</v>
+        <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>21</v>
+        <v>1</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B2">
-        <v>1.8772</v>
+        <v>2.8157999999999999</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
-        <v>16</v>
+        <v>3</v>
       </c>
       <c r="B3">
-        <v>2.8157999999999999</v>
+        <v>3.7544</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="B4">
-        <v>1.8772</v>
+        <v>2.8157999999999999</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
-        <v>17</v>
+        <v>5</v>
       </c>
       <c r="B5">
-        <v>2.8157999999999999</v>
+        <v>1.7290000000000001</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="B6">
-        <v>1.7290000000000001</v>
+        <v>4.5599999999999996</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
-        <v>2</v>
+        <v>7</v>
       </c>
       <c r="B7">
-        <v>2.8157999999999999</v>
+        <v>4.6929999999999996</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
-        <v>3</v>
+        <v>8</v>
       </c>
       <c r="B8">
-        <v>1.8772</v>
+        <v>6.5701999999999998</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
-        <v>4</v>
+        <v>9</v>
       </c>
       <c r="B9">
-        <v>2.3464999999999998</v>
-      </c>
-    </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A10" t="s">
-        <v>5</v>
-      </c>
-      <c r="B10">
-        <v>3.2850999999999999</v>
-      </c>
-    </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A11" t="s">
-        <v>6</v>
-      </c>
-      <c r="B11">
-        <v>1.8772</v>
-      </c>
-    </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A12" t="s">
-        <v>7</v>
-      </c>
-      <c r="B12">
-        <v>3.7544</v>
-      </c>
-    </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A13" t="s">
-        <v>8</v>
-      </c>
-      <c r="B13">
-        <v>2.8157999999999999</v>
-      </c>
-    </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A14" t="s">
-        <v>9</v>
-      </c>
-      <c r="B14">
-        <v>3.2850999999999999</v>
-      </c>
-    </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A15" t="s">
-        <v>10</v>
-      </c>
-      <c r="B15">
-        <v>2.3464999999999998</v>
-      </c>
-    </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A16" t="s">
-        <v>11</v>
-      </c>
-      <c r="B16">
-        <v>4.2237</v>
-      </c>
-    </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A17" t="s">
-        <v>12</v>
-      </c>
-      <c r="B17">
-        <v>4.6929999999999996</v>
-      </c>
-    </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A18" t="s">
-        <v>13</v>
-      </c>
-      <c r="B18">
-        <v>3.7544</v>
-      </c>
-    </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A19" t="s">
-        <v>14</v>
-      </c>
-      <c r="B19">
-        <v>2.8157999999999999</v>
-      </c>
-    </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A20" t="s">
-        <v>15</v>
-      </c>
-      <c r="B20">
-        <v>4.5599999999999996</v>
-      </c>
-    </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A21" t="s">
-        <v>18</v>
-      </c>
-      <c r="B21">
-        <v>6.5701999999999998</v>
-      </c>
-    </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A22" t="s">
-        <v>19</v>
-      </c>
-      <c r="B22">
         <v>7.0395000000000003</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Added some node attributes as well as processed some graph queries
</commit_message>
<xml_diff>
--- a/DeepRL/Data/stdcell45nm.xlsx
+++ b/DeepRL/Data/stdcell45nm.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\Projects\Automate Chip Design Using ML and DL\Model Work\DeepRL\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DD990174-AC43-451F-9D1B-C19814172949}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{73029426-0A5D-4C1A-9F59-725BD235BA56}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,13 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
-  <si>
-    <t>MACROS</t>
-  </si>
-  <si>
-    <t>AREA</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="14">
   <si>
     <t>nand</t>
   </si>
@@ -57,10 +51,22 @@
     <t>fflopd</t>
   </si>
   <si>
-    <t>fflond</t>
-  </si>
-  <si>
     <t>nor</t>
+  </si>
+  <si>
+    <t>p1_cap</t>
+  </si>
+  <si>
+    <t>l_power</t>
+  </si>
+  <si>
+    <t>area</t>
+  </si>
+  <si>
+    <t>macro</t>
+  </si>
+  <si>
+    <t>p2_cap</t>
   </si>
 </sst>
 </file>
@@ -378,100 +384,182 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:B11"/>
+  <dimension ref="A1:E10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A6" sqref="A6"/>
+      <selection activeCell="F14" sqref="F14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B1" t="s">
+        <v>11</v>
+      </c>
+      <c r="C1" t="s">
+        <v>10</v>
+      </c>
+      <c r="D1" t="s">
+        <v>9</v>
+      </c>
+      <c r="E1" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A2" t="s">
+        <v>4</v>
+      </c>
+      <c r="B2">
+        <v>1.0640000000000001</v>
+      </c>
+      <c r="C2">
+        <v>25.07</v>
+      </c>
+      <c r="D2">
+        <v>0.91810000000000003</v>
+      </c>
+      <c r="E2">
+        <v>0.97460000000000002</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A3" t="s">
+        <v>1</v>
+      </c>
+      <c r="B3">
+        <v>1.0640000000000001</v>
+      </c>
+      <c r="C3">
+        <v>22.69</v>
+      </c>
+      <c r="D3">
+        <v>0.94679999999999997</v>
+      </c>
+      <c r="E3">
+        <v>0.94189999999999996</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A4" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A2" t="s">
+      <c r="B4">
+        <v>0.79800000000000004</v>
+      </c>
+      <c r="C4">
+        <v>17.39</v>
+      </c>
+      <c r="D4">
+        <v>1.599</v>
+      </c>
+      <c r="E4">
+        <v>1.6641999999999999</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A5" t="s">
+        <v>8</v>
+      </c>
+      <c r="B5">
+        <v>0.79800000000000004</v>
+      </c>
+      <c r="C5">
+        <v>21.2</v>
+      </c>
+      <c r="D5">
+        <v>1.7144999999999999</v>
+      </c>
+      <c r="E5">
+        <v>1.6513</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A6" t="s">
+        <v>3</v>
+      </c>
+      <c r="B6">
+        <v>0.53200000000000003</v>
+      </c>
+      <c r="C6">
+        <v>14.35</v>
+      </c>
+      <c r="D6">
+        <v>1.7001999999999999</v>
+      </c>
+      <c r="E6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A7" t="s">
+        <v>5</v>
+      </c>
+      <c r="B7">
+        <v>1.5960000000000001</v>
+      </c>
+      <c r="C7">
+        <v>36.159999999999997</v>
+      </c>
+      <c r="D7">
+        <v>2.2321</v>
+      </c>
+      <c r="E7">
+        <v>2.4115000000000002</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A8" t="s">
+        <v>6</v>
+      </c>
+      <c r="B8">
+        <v>1.5960000000000001</v>
+      </c>
+      <c r="C8">
+        <v>36.44</v>
+      </c>
+      <c r="D8">
+        <v>2.2328000000000001</v>
+      </c>
+      <c r="E8">
+        <v>2.5735999999999999</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A9" t="s">
+        <v>7</v>
+      </c>
+      <c r="B9">
+        <v>4.5220000000000002</v>
+      </c>
+      <c r="C9">
+        <v>79.11</v>
+      </c>
+      <c r="D9">
+        <v>0.94969999999999999</v>
+      </c>
+      <c r="E9">
+        <v>1.1403000000000001</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A10" t="s">
         <v>2</v>
       </c>
-      <c r="B2">
-        <v>3.2850999999999999</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A3" t="s">
-        <v>3</v>
-      </c>
-      <c r="B3">
-        <v>3.2850999999999999</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A4" t="s">
-        <v>4</v>
-      </c>
-      <c r="B4">
-        <v>3.2850999999999999</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A5" t="s">
-        <v>5</v>
-      </c>
-      <c r="B5">
-        <v>3.2850999999999999</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A6" t="s">
-        <v>6</v>
-      </c>
-      <c r="B6">
-        <v>3.2850999999999999</v>
-      </c>
-    </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A7" t="s">
-        <v>11</v>
-      </c>
-      <c r="B7">
-        <v>4.6929999999999996</v>
-      </c>
-    </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A8" t="s">
-        <v>9</v>
-      </c>
-      <c r="B8">
-        <v>7.0395000000000003</v>
-      </c>
-    </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A9" t="s">
-        <v>10</v>
-      </c>
-      <c r="B9">
-        <v>7.0385</v>
-      </c>
-    </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A10" t="s">
-        <v>7</v>
-      </c>
       <c r="B10">
-        <v>4.2237</v>
-      </c>
-    </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A11" t="s">
-        <v>8</v>
-      </c>
-      <c r="B11">
-        <v>4.2237</v>
+        <v>0.79800000000000004</v>
+      </c>
+      <c r="C10">
+        <v>21.44</v>
+      </c>
+      <c r="D10">
+        <v>0.97470000000000001</v>
+      </c>
+      <c r="E10">
+        <v>0</v>
       </c>
     </row>
   </sheetData>

</xml_diff>